<commit_message>
fix: added cip dummy report
</commit_message>
<xml_diff>
--- a/reports/cip_management_report/CIP Dummy Report.xlsx
+++ b/reports/cip_management_report/CIP Dummy Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\Lumo_reports\reports\cip_management_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EE1F93-744D-4355-A495-4EA92D1A3F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869BA6C0-DFCD-4D36-A3FE-312E1B53C009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ECE2B712-0DE4-41CA-92B5-F54CE8EA74E4}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="134">
   <si>
     <t>Deal Pipeline</t>
   </si>
@@ -427,6 +427,21 @@
   </si>
   <si>
     <t>* Won is negative as leaves the pipeline once won</t>
+  </si>
+  <si>
+    <t>€260m</t>
+  </si>
+  <si>
+    <t>€870m</t>
+  </si>
+  <si>
+    <t>€675m</t>
+  </si>
+  <si>
+    <t>€1175m</t>
+  </si>
+  <si>
+    <t>€1490m</t>
   </si>
 </sst>
 </file>
@@ -612,7 +627,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -717,6 +732,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -7073,14 +7096,349 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB4B7AF-F240-4D01-87EF-D6DBAFF280DF}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="52" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="50"/>
+      <c r="C3" s="10"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="3">
+        <v>5600</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="12">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="54"/>
+      <c r="C6" s="55"/>
+    </row>
+    <row r="8" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B8" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="50"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="52" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="52" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="52" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="52" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="52" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="53" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="B18" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K18" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="M18" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="15">
+        <v>2440</v>
+      </c>
+      <c r="C19" s="16">
+        <v>0.43571428571428572</v>
+      </c>
+      <c r="D19" s="16">
+        <v>0.20333333333333328</v>
+      </c>
+      <c r="E19" s="21">
+        <v>138.67233606557375</v>
+      </c>
+      <c r="F19" s="18">
+        <v>135.61065573770492</v>
+      </c>
+      <c r="G19" s="18">
+        <v>130.61065573770492</v>
+      </c>
+      <c r="H19" s="22">
+        <v>13.867233606557376</v>
+      </c>
+      <c r="I19" s="18">
+        <v>13.471311475409836</v>
+      </c>
+      <c r="J19" s="18">
+        <v>13.678278688524593</v>
+      </c>
+      <c r="K19" s="22">
+        <v>4.0163934426229506</v>
+      </c>
+      <c r="L19" s="18">
+        <v>4.2889344262295088</v>
+      </c>
+      <c r="M19" s="18">
+        <v>4.7274590163934436</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C23"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="24">
+        <v>5</v>
+      </c>
+      <c r="D24" s="24">
+        <v>20</v>
+      </c>
+      <c r="E24" s="24">
+        <v>50</v>
+      </c>
+      <c r="F24" s="24">
+        <v>75</v>
+      </c>
+      <c r="G24" s="24">
+        <v>90</v>
+      </c>
+      <c r="H24" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="43">
+        <v>20</v>
+      </c>
+      <c r="D25" s="44">
+        <v>1654.1</v>
+      </c>
+      <c r="E25" s="44">
+        <v>1570</v>
+      </c>
+      <c r="F25" s="44">
+        <v>75</v>
+      </c>
+      <c r="G25" s="44">
+        <v>203.3</v>
+      </c>
+      <c r="H25" s="44">
+        <v>3522.4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="37"/>
+      <c r="D26" s="38">
+        <v>2006</v>
+      </c>
+      <c r="E26" s="38">
+        <v>282</v>
+      </c>
+      <c r="F26" s="38">
+        <v>250</v>
+      </c>
+      <c r="G26" s="38">
+        <v>157.4</v>
+      </c>
+      <c r="H26" s="38">
+        <v>2695.4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="40"/>
+      <c r="D27" s="41">
+        <v>30</v>
+      </c>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="37"/>
+      <c r="D28" s="38">
+        <v>3729.03</v>
+      </c>
+      <c r="E28" s="38">
+        <v>543.5</v>
+      </c>
+      <c r="F28" s="38">
+        <v>102.5</v>
+      </c>
+      <c r="G28" s="38">
+        <v>1365.5</v>
+      </c>
+      <c r="H28" s="38">
+        <v>5740.53</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="26">
+        <v>126</v>
+      </c>
+      <c r="E29" s="26">
+        <v>25</v>
+      </c>
+      <c r="F29" s="26">
+        <v>5</v>
+      </c>
+      <c r="G29" s="26">
+        <v>15</v>
+      </c>
+      <c r="H29" s="35">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="29">
+        <v>20</v>
+      </c>
+      <c r="D30" s="30">
+        <v>8236.6299999999992</v>
+      </c>
+      <c r="E30" s="30">
+        <v>2452</v>
+      </c>
+      <c r="F30" s="30">
+        <v>454.5</v>
+      </c>
+      <c r="G30" s="30">
+        <v>1792.2</v>
+      </c>
+      <c r="H30" s="30">
+        <v>12955.33</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7090,7 +7448,7 @@
   <dimension ref="B2:V45"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7628,7 +7986,7 @@
   <dimension ref="B2:P33"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+      <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8937,7 +9295,7 @@
   <dimension ref="B2:O66"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+      <selection activeCell="B4" sqref="B4:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>